<commit_message>
creating file with feature descriptions of compas dataset
</commit_message>
<xml_diff>
--- a/datasets/compas/colunas datasets.xlsx
+++ b/datasets/compas/colunas datasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Área de Trabalho\compas-dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Downloads\Temporario\fairness-testing\datasets\compas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE266BFF-0E66-49D6-B59E-F4245F3CC79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3837A3A-1F24-4C11-AE2D-6CF1BED834BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="145">
   <si>
     <t>cox-violent-parsed:</t>
   </si>
@@ -354,9 +354,6 @@
     <t>raça</t>
   </si>
   <si>
-    <t>nível de decisão de reincidência</t>
-  </si>
-  <si>
     <t>data da prisão</t>
   </si>
   <si>
@@ -369,7 +366,100 @@
     <t>dias de prisão na triagem</t>
   </si>
   <si>
-    <t>e é reincidente</t>
+    <t>nível de decisão de reincidência (de 1 a 10)</t>
+  </si>
+  <si>
+    <t>nível de decisão de reincidência violenta (de 1 a 10)</t>
+  </si>
+  <si>
+    <t>índice de decisão de reincidência (baixo, médio, alto)</t>
+  </si>
+  <si>
+    <t>se é reincidente</t>
+  </si>
+  <si>
+    <t>grau de acusação</t>
+  </si>
+  <si>
+    <t>CO3</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>MO3</t>
+  </si>
+  <si>
+    <t>NI0</t>
+  </si>
+  <si>
+    <t>TCX</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>c_charge_degree: https://www.davidcohenlawfirm.com/pennsylvania-crime-classification</t>
+  </si>
+  <si>
+    <t>Murder Offense</t>
+  </si>
+  <si>
+    <t>Felony Crime 1º degree</t>
+  </si>
+  <si>
+    <t>Felony Crime 2º degree</t>
+  </si>
+  <si>
+    <t>Felony Crime 3º degree</t>
+  </si>
+  <si>
+    <t>Felony Crime 5º degree</t>
+  </si>
+  <si>
+    <t>Felony Crime 6º degree</t>
+  </si>
+  <si>
+    <t>Felony Crime 7º degree</t>
+  </si>
+  <si>
+    <t>Misdemeanors 1º degree</t>
+  </si>
+  <si>
+    <t>Misdemeanors 2º degree</t>
+  </si>
+  <si>
+    <t>data de aniversário (date of birthday)</t>
+  </si>
+  <si>
+    <t>data de ocorrência do crime</t>
+  </si>
+  <si>
+    <t>número de identificação do caso</t>
   </si>
 </sst>
 </file>
@@ -418,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,6 +527,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,881 +817,1085 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G58"/>
+  <dimension ref="B1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="1"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K2" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K6" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K11" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K12" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K13" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K14" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+      <c r="K15" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="K16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1"/>
+      <c r="D32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1"/>
+      <c r="D34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1"/>
+      <c r="D39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="1"/>
+      <c r="D40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="1"/>
+      <c r="D41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="1"/>
+      <c r="D42" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="1"/>
+      <c r="D44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="1"/>
+      <c r="D47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="1"/>
+      <c r="D48" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="1"/>
+      <c r="D50" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="1"/>
+      <c r="D51" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="1"/>
+      <c r="D52" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="3" t="s">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D55" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
+      <c r="E57" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>